<commit_message>
Adding a test import spreadsheet
</commit_message>
<xml_diff>
--- a/test_data/import_template_EXAMPLE.xlsx
+++ b/test_data/import_template_EXAMPLE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="515">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -676,6 +676,9 @@
     <t xml:space="preserve">alice.smith@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">alice.smith</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alice</t>
   </si>
   <si>
@@ -694,6 +697,9 @@
     <t xml:space="preserve">bob.smith@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">bob.smith</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bob</t>
   </si>
   <si>
@@ -703,6 +709,9 @@
     <t xml:space="preserve">charlie.smith@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">charlie.smith</t>
+  </si>
+  <si>
     <t xml:space="preserve">Charlie</t>
   </si>
   <si>
@@ -712,6 +721,9 @@
     <t xml:space="preserve">diana.smith@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">diana.smith</t>
+  </si>
+  <si>
     <t xml:space="preserve">Diana</t>
   </si>
   <si>
@@ -724,6 +736,9 @@
     <t xml:space="preserve">eve.smith@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">eve.smith</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eve</t>
   </si>
   <si>
@@ -733,6 +748,9 @@
     <t xml:space="preserve">frank.smith@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">frank.smith</t>
+  </si>
+  <si>
     <t xml:space="preserve">Frank</t>
   </si>
   <si>
@@ -742,6 +760,9 @@
     <t xml:space="preserve">jos.garca@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">jos.garca</t>
+  </si>
+  <si>
     <t xml:space="preserve">José</t>
   </si>
   <si>
@@ -754,6 +775,9 @@
     <t xml:space="preserve">ana.garca@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">ana.garca</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ana</t>
   </si>
   <si>
@@ -763,6 +787,9 @@
     <t xml:space="preserve">marta.garca@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">marta.garca</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marta</t>
   </si>
   <si>
@@ -772,6 +799,9 @@
     <t xml:space="preserve">sven.mller@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">sven.mller</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sven</t>
   </si>
   <si>
@@ -784,6 +814,9 @@
     <t xml:space="preserve">ke.mller@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">ke.mller</t>
+  </si>
+  <si>
     <t xml:space="preserve">Åke</t>
   </si>
   <si>
@@ -793,6 +826,9 @@
     <t xml:space="preserve">la.mller@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">la.mller</t>
+  </si>
+  <si>
     <t xml:space="preserve">Léa</t>
   </si>
   <si>
@@ -802,6 +838,9 @@
     <t xml:space="preserve">noor.imi@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">noor.imi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Noor</t>
   </si>
   <si>
@@ -814,6 +853,9 @@
     <t xml:space="preserve">priya.imi@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">priya.imi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Priya</t>
   </si>
   <si>
@@ -823,6 +865,9 @@
     <t xml:space="preserve">hana.imi@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">hana.imi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hana</t>
   </si>
   <si>
@@ -832,6 +877,9 @@
     <t xml:space="preserve">trent.oneil@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">trent.oneil</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trent</t>
   </si>
   <si>
@@ -844,6 +892,9 @@
     <t xml:space="preserve">victor.oneil@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">victor.oneil</t>
+  </si>
+  <si>
     <t xml:space="preserve">Victor</t>
   </si>
   <si>
@@ -853,6 +904,9 @@
     <t xml:space="preserve">walter.oneil@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">walter.oneil</t>
+  </si>
+  <si>
     <t xml:space="preserve">Walter</t>
   </si>
   <si>
@@ -862,6 +916,9 @@
     <t xml:space="preserve">ken.lee@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">ken.lee</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ken</t>
   </si>
   <si>
@@ -874,6 +931,9 @@
     <t xml:space="preserve">laura.lee@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">laura.lee</t>
+  </si>
+  <si>
     <t xml:space="preserve">Laura</t>
   </si>
   <si>
@@ -883,6 +943,9 @@
     <t xml:space="preserve">mallory.lee@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">mallory.lee</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mallory</t>
   </si>
   <si>
@@ -892,6 +955,9 @@
     <t xml:space="preserve">niaj.lee@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">niaj.lee</t>
+  </si>
+  <si>
     <t xml:space="preserve">Niaj</t>
   </si>
   <si>
@@ -901,6 +967,9 @@
     <t xml:space="preserve">peggy.jones@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">peggy.jones</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peggy</t>
   </si>
   <si>
@@ -913,6 +982,9 @@
     <t xml:space="preserve">ana.snchez@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">ana.snchez</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sánchez</t>
   </si>
   <si>
@@ -922,6 +994,9 @@
     <t xml:space="preserve">heidi.wilson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">heidi.wilson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Heidi</t>
   </si>
   <si>
@@ -934,6 +1009,9 @@
     <t xml:space="preserve">eve.johnson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">eve.johnson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Johnson</t>
   </si>
   <si>
@@ -943,6 +1021,9 @@
     <t xml:space="preserve">ke.hernandez@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">ke.hernandez</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hernandez</t>
   </si>
   <si>
@@ -952,6 +1033,9 @@
     <t xml:space="preserve">sven.martin@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">sven.martin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Martin</t>
   </si>
   <si>
@@ -961,6 +1045,9 @@
     <t xml:space="preserve">noor.kaur@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">noor.kaur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kaur</t>
   </si>
   <si>
@@ -970,6 +1057,9 @@
     <t xml:space="preserve">hkon.imi@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">hkon.imi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Håkon</t>
   </si>
   <si>
@@ -979,6 +1069,9 @@
     <t xml:space="preserve">wei.kuznetsov@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">wei.kuznetsov</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wei</t>
   </si>
   <si>
@@ -991,6 +1084,9 @@
     <t xml:space="preserve">mei.imi@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">mei.imi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mei</t>
   </si>
   <si>
@@ -1000,6 +1096,9 @@
     <t xml:space="preserve">peggy.anderson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">peggy.anderson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anderson</t>
   </si>
   <si>
@@ -1009,6 +1108,9 @@
     <t xml:space="preserve">mllertest.anderson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">mllertest.anderson</t>
+  </si>
+  <si>
     <t xml:space="preserve">MüllerTest</t>
   </si>
   <si>
@@ -1018,6 +1120,9 @@
     <t xml:space="preserve">grace.miller@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">grace.miller</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grace</t>
   </si>
   <si>
@@ -1030,6 +1135,9 @@
     <t xml:space="preserve">rupert.ivanov@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">rupert.ivanov</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rupert</t>
   </si>
   <si>
@@ -1042,6 +1150,9 @@
     <t xml:space="preserve">xavier.miller@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">xavier.miller</t>
+  </si>
+  <si>
     <t xml:space="preserve">Xavier</t>
   </si>
   <si>
@@ -1051,6 +1162,9 @@
     <t xml:space="preserve">zo.kaur@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">zo.kaur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zoë</t>
   </si>
   <si>
@@ -1060,6 +1174,9 @@
     <t xml:space="preserve">wei.harris@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">wei.harris</t>
+  </si>
+  <si>
     <t xml:space="preserve">Harris</t>
   </si>
   <si>
@@ -1069,12 +1186,18 @@
     <t xml:space="preserve">ke.wilson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">ke.wilson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Åke	Wilson</t>
   </si>
   <si>
     <t xml:space="preserve">olivia.gonzalez@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">olivia.gonzalez</t>
+  </si>
+  <si>
     <t xml:space="preserve">Olivia</t>
   </si>
   <si>
@@ -1087,30 +1210,45 @@
     <t xml:space="preserve">heidi.anderson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">heidi.anderson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Heidi	Anderson</t>
   </si>
   <si>
     <t xml:space="preserve">jos.hernandez@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">jos.hernandez</t>
+  </si>
+  <si>
     <t xml:space="preserve">José	Hernandez</t>
   </si>
   <si>
     <t xml:space="preserve">eve.martin@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">eve.martin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eve	Martin</t>
   </si>
   <si>
     <t xml:space="preserve">trent.kaur@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">trent.kaur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trent	Kaur</t>
   </si>
   <si>
     <t xml:space="preserve">trent.lopez@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">trent.lopez</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lopez</t>
   </si>
   <si>
@@ -1120,36 +1258,54 @@
     <t xml:space="preserve">trent.ivanov@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">trent.ivanov</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trent	Ivanov</t>
   </si>
   <si>
     <t xml:space="preserve">charlie.wilson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">charlie.wilson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Charlie	Wilson</t>
   </si>
   <si>
     <t xml:space="preserve">sven.wilson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">sven.wilson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sven	Wilson</t>
   </si>
   <si>
     <t xml:space="preserve">heidi.mller@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">heidi.mller</t>
+  </si>
+  <si>
     <t xml:space="preserve">Heidi	Müller</t>
   </si>
   <si>
     <t xml:space="preserve">ken.imi@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">ken.imi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ken	Šimić</t>
   </si>
   <si>
     <t xml:space="preserve">eve.taylor@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">eve.taylor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Taylor</t>
   </si>
   <si>
@@ -1159,18 +1315,27 @@
     <t xml:space="preserve">eve.harris@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">eve.harris</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eve	Harris</t>
   </si>
   <si>
     <t xml:space="preserve">alice.lee@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">alice.lee</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alice	Lee</t>
   </si>
   <si>
     <t xml:space="preserve">sybil.snchez@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">sybil.snchez</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sybil</t>
   </si>
   <si>
@@ -1180,24 +1345,36 @@
     <t xml:space="preserve">mei.smith@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">mei.smith</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mei	SMITH</t>
   </si>
   <si>
     <t xml:space="preserve">walter.martin@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">walter.martin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Walter	Martin</t>
   </si>
   <si>
     <t xml:space="preserve">priya.anderson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">priya.anderson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Priya	Anderson</t>
   </si>
   <si>
     <t xml:space="preserve">hana.thompson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">hana.thompson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thompson</t>
   </si>
   <si>
@@ -1207,6 +1384,9 @@
     <t xml:space="preserve">yvonne.chen@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">yvonne.chen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yvonne</t>
   </si>
   <si>
@@ -1219,12 +1399,18 @@
     <t xml:space="preserve">zo.mller@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">zo.mller</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zoë	Müller</t>
   </si>
   <si>
     <t xml:space="preserve">mei.thomas@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">mei.thomas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thomas</t>
   </si>
   <si>
@@ -1234,6 +1420,9 @@
     <t xml:space="preserve">hkon.jackson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">hkon.jackson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jackson</t>
   </si>
   <si>
@@ -1243,30 +1432,45 @@
     <t xml:space="preserve">frank.wilson@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">frank.wilson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Frank	Wilson</t>
   </si>
   <si>
     <t xml:space="preserve">trent.gonzalez@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">trent.gonzalez</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trent	Gonzalez</t>
   </si>
   <si>
     <t xml:space="preserve">priya.thomas@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">priya.thomas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Priya	Thomas</t>
   </si>
   <si>
     <t xml:space="preserve">la.thomas@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">la.thomas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Léa	Thomas</t>
   </si>
   <si>
     <t xml:space="preserve">li.miller@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">li.miller</t>
+  </si>
+  <si>
     <t xml:space="preserve">Li</t>
   </si>
   <si>
@@ -1276,24 +1480,36 @@
     <t xml:space="preserve">hana.taylor@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">hana.taylor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hana	Taylor</t>
   </si>
   <si>
     <t xml:space="preserve">sven.kuznetsov@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">sven.kuznetsov</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sven	Kuznetsov</t>
   </si>
   <si>
     <t xml:space="preserve">heidi.kaur@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">heidi.kaur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Heidi	Kaur</t>
   </si>
   <si>
     <t xml:space="preserve">victor.williams@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">victor.williams</t>
+  </si>
+  <si>
     <t xml:space="preserve">Williams</t>
   </si>
   <si>
@@ -1303,6 +1519,9 @@
     <t xml:space="preserve">wei.brown@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">wei.brown</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brown</t>
   </si>
   <si>
@@ -1312,12 +1531,18 @@
     <t xml:space="preserve">eve.gonzalez@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">eve.gonzalez</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eve	Gonzalez</t>
   </si>
   <si>
     <t xml:space="preserve">judy.brown@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">judy.brown</t>
+  </si>
+  <si>
     <t xml:space="preserve">Judy</t>
   </si>
   <si>
@@ -1327,10 +1552,16 @@
     <t xml:space="preserve">sybil.ivanov@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">sybil.ivanov</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sybil	Ivanov</t>
   </si>
   <si>
     <t xml:space="preserve">hana.smith@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hana.smith</t>
   </si>
   <si>
     <t xml:space="preserve">Hana	SMITH</t>
@@ -1634,14 +1865,14 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E95" activeCellId="0" sqref="E95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A101" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B135" activeCellId="0" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.66"/>
@@ -1789,7 +2020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="str">
         <f aca="false">"test"&amp;ROW(A7)+0&amp;"@test.com"</f>
         <v>test7@test.com</v>
@@ -1897,7 +2128,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="str">
         <f aca="false">"test"&amp;ROW(A13)+0&amp;"@test.com"</f>
         <v>test13@test.com</v>
@@ -2005,7 +2236,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="str">
         <f aca="false">"test"&amp;ROW(A19)+0&amp;"@test.com"</f>
         <v>test19@test.com</v>
@@ -2636,1123 +2867,1363 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>219</v>
       </c>
+      <c r="D56" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="E56" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="D57" s="0" t="s">
+      <c r="E57" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="E61" s="1" t="s">
+      <c r="D111" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="E113" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C63" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="D115" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C64" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="C69" s="0" t="s">
+      <c r="D122" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D69" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="E75" s="1" t="s">
+      <c r="D128" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="D80" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="D81" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="D88" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="D89" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="D90" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="D91" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="D92" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>340</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="C96" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="D96" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="C97" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="D97" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>351</v>
-      </c>
-      <c r="D98" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="C99" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="D99" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="C100" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="D100" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
-        <v>358</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="C102" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="D102" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="C103" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="D103" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>365</v>
-      </c>
-      <c r="C104" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="D104" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="C105" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="D105" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="C106" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="D106" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="C107" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="D107" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="C108" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="D108" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="C109" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="D109" s="0" t="s">
-        <v>376</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="C110" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="D110" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
-        <v>380</v>
-      </c>
-      <c r="C111" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="D111" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
-        <v>382</v>
-      </c>
-      <c r="C112" s="0" t="s">
-        <v>383</v>
-      </c>
-      <c r="D112" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="C113" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="D113" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
-        <v>387</v>
-      </c>
-      <c r="C114" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="D114" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="C115" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="D115" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>389</v>
-      </c>
-      <c r="C116" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="D116" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="C117" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="D117" s="0" t="s">
-        <v>392</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
-        <v>394</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="D118" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="C119" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="D119" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C120" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="D120" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
-        <v>403</v>
-      </c>
-      <c r="C121" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="D121" s="0" t="s">
-        <v>404</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="C122" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="D122" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
-        <v>408</v>
-      </c>
-      <c r="C123" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="D123" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="C124" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="D124" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
-        <v>412</v>
-      </c>
-      <c r="C125" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="D125" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
-        <v>414</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>415</v>
-      </c>
-      <c r="D126" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
-        <v>417</v>
-      </c>
-      <c r="C127" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="D127" s="0" t="s">
-        <v>376</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
-        <v>419</v>
-      </c>
-      <c r="C128" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="D128" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
-        <v>421</v>
-      </c>
-      <c r="C129" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="D129" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
-        <v>423</v>
-      </c>
-      <c r="C130" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="D130" s="0" t="s">
-        <v>424</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
-        <v>426</v>
-      </c>
-      <c r="C131" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="D131" s="0" t="s">
-        <v>427</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
-        <v>429</v>
-      </c>
-      <c r="C132" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="D132" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>432</v>
-      </c>
-      <c r="D133" s="0" t="s">
-        <v>427</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
-        <v>434</v>
-      </c>
-      <c r="C134" s="0" t="s">
-        <v>383</v>
-      </c>
-      <c r="D134" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
-        <v>436</v>
-      </c>
-      <c r="C135" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="D135" s="0" t="s">
-        <v>231</v>
+      <c r="D135" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>437</v>
+        <v>514</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>